<commit_message>
actualizacion 12 11 2019
</commit_message>
<xml_diff>
--- a/src/main/resources/com/relative/QuskiOro/Matrices/Constantes.xlsx
+++ b/src/main/resources/com/relative/QuskiOro/Matrices/Constantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4168ccd2be4a7b9a/Desktop/NOVACIONES 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_49CF470B67224160BFB4670EAFF9BA6CAAF98643" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FF544E5F-A9D7-488A-ACB6-91A426900E6F}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_49CF470B67224160BFB4670EAFF9BA6CAAF98643" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{66E4A88A-B16C-416D-B825-552F42C600B2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
   <si>
     <t>RuleSet</t>
   </si>
@@ -215,24 +215,12 @@
     <t>CodigoErrorSinGarantia,1</t>
   </si>
   <si>
-    <t>MENSAJE DE ERROR SIN GARANTIA</t>
-  </si>
-  <si>
-    <t>MensajeErrorSinGarantia,Lo sentimos no fue posible generar ofertas.</t>
-  </si>
-  <si>
     <t>CCODIGO ERROR VALORES NO CUADRAN</t>
   </si>
   <si>
     <t>CodigoErrorValoresCreditoNoCuadran,1</t>
   </si>
   <si>
-    <t>MENSAJE DE ERROR VALORES NO CUADRAN</t>
-  </si>
-  <si>
-    <t>MensajeErrorValoresCreditoNoCuadran,DATOS DE CREDITO NO CUADRAN</t>
-  </si>
-  <si>
     <t>CODIGO DE TIPO CREDITO CUOTA</t>
   </si>
   <si>
@@ -285,6 +273,12 @@
   </si>
   <si>
     <t>ListaPlazosMontoFinanciadoNovacion,13</t>
+  </si>
+  <si>
+    <t>CodigoErrorGarantiasNoCuadran,1</t>
+  </si>
+  <si>
+    <t>CodigoErrorGarantiaNovacionDistinta,1</t>
   </si>
 </sst>
 </file>
@@ -543,7 +537,7 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1424940</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -592,7 +586,7 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1424940</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -933,7 +927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
@@ -1198,14 +1192,14 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E22" s="8"/>
     </row>
@@ -1287,7 +1281,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>50</v>
       </c>
@@ -1309,11 +1303,11 @@
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>54</v>
       </c>
@@ -1322,7 +1316,7 @@
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="8" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1375,12 +1369,12 @@
       <c r="C35" s="11"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>12</v>
@@ -1388,12 +1382,12 @@
       <c r="C36" s="11"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>12</v>
@@ -1406,28 +1400,28 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="8"/>
-      <c r="E38" s="8" t="s">
-        <v>68</v>
+      <c r="E38" s="12" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="8"/>
-      <c r="E39" s="8" t="s">
-        <v>73</v>
+      <c r="E39" s="12" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>